<commit_message>
further tweaking the overall structure of lib
</commit_message>
<xml_diff>
--- a/Assets/Vendor/DataHelpers/Editor/Tests/Fixtures/TestData.xlsx
+++ b/Assets/Vendor/DataHelpers/Editor/Tests/Fixtures/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12360"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12360" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Foo" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>#author</t>
   </si>
   <si>
-    <t>Nick</t>
-  </si>
-  <si>
     <t>#description</t>
   </si>
   <si>
@@ -40,12 +37,6 @@
     <t>[Baz]</t>
   </si>
   <si>
-    <t>Bar test data</t>
-  </si>
-  <si>
-    <t>Foo test data</t>
-  </si>
-  <si>
     <t>$foo2</t>
   </si>
   <si>
@@ -56,6 +47,12 @@
   </si>
   <si>
     <t>$bar2</t>
+  </si>
+  <si>
+    <t>foo description</t>
+  </si>
+  <si>
+    <t>foo author</t>
   </si>
 </sst>
 </file>
@@ -412,8 +409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -423,15 +420,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -440,7 +437,7 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1">
         <v>100</v>
@@ -448,7 +445,7 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
         <v>200</v>
@@ -457,13 +454,13 @@
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -497,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -512,15 +509,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -529,7 +526,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
         <v>300</v>
@@ -537,7 +534,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1">
         <v>400</v>
@@ -545,13 +542,13 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>